<commit_message>
Update DACD w/ state downscale
</commit_message>
<xml_diff>
--- a/InputData/geoeng/DACD/Direct Air Capture Data.xlsx
+++ b/InputData/geoeng/DACD/Direct Air Capture Data.xlsx
@@ -1,34 +1,45 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11213"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox (Energy Innovation)\Desktop\eps-us develop DACD\InputData\geoeng\DACD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nathaniyer/Library/Containers/com.microsoft.Excel/Data/state-eps-data-repository/CO/geoeng/DACD/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5D759AB7-ACAB-D44C-81DD-FEFD03ADBD3B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23415" windowHeight="10875"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="23420" windowHeight="15740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="Data" sheetId="2" r:id="rId2"/>
-    <sheet name="DACD-potential" sheetId="3" r:id="rId3"/>
-    <sheet name="DACD-energyintensity" sheetId="5" r:id="rId4"/>
-    <sheet name="DACD-capex" sheetId="6" r:id="rId5"/>
+    <sheet name="State Downscale" sheetId="7" r:id="rId3"/>
+    <sheet name="DACD-potential" sheetId="3" r:id="rId4"/>
+    <sheet name="DACD-energyintensity" sheetId="5" r:id="rId5"/>
+    <sheet name="DACD-capex" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="214">
   <si>
     <t>Sources:</t>
   </si>
@@ -289,17 +300,398 @@
   </si>
   <si>
     <t>Amortized CapEx and OM Cost Notes</t>
+  </si>
+  <si>
+    <t>State by State GDP (for downscaling, 2019)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://apps.bea.gov/itable/iTable.cfm?ReqID=70&amp;step=1#reqid=70&amp;step=1&amp;isuri=1 </t>
+  </si>
+  <si>
+    <t>SAGDP1 Gross Domestic Product (GDP) summary, annual by state</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Real Gross Domestic Product (GDP) (Millions of chained 2012 dollars) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bureau of Economic Analysis </t>
+  </si>
+  <si>
+    <t>State or DC</t>
+  </si>
+  <si>
+    <t>GeoFips</t>
+  </si>
+  <si>
+    <t>GeoName</t>
+  </si>
+  <si>
+    <t>United States</t>
+  </si>
+  <si>
+    <t>Alabama</t>
+  </si>
+  <si>
+    <t>Alaska</t>
+  </si>
+  <si>
+    <t>Arizona</t>
+  </si>
+  <si>
+    <t>Arkansas</t>
+  </si>
+  <si>
+    <t>California</t>
+  </si>
+  <si>
+    <t>Colorado</t>
+  </si>
+  <si>
+    <t>Connecticut</t>
+  </si>
+  <si>
+    <t>Delaware</t>
+  </si>
+  <si>
+    <t>District of Columbia</t>
+  </si>
+  <si>
+    <t>Florida</t>
+  </si>
+  <si>
+    <t>Georgia</t>
+  </si>
+  <si>
+    <t>Hawaii</t>
+  </si>
+  <si>
+    <t>Idaho</t>
+  </si>
+  <si>
+    <t>Illinois</t>
+  </si>
+  <si>
+    <t>Indiana</t>
+  </si>
+  <si>
+    <t>Iowa</t>
+  </si>
+  <si>
+    <t>Kansas</t>
+  </si>
+  <si>
+    <t>Kentucky</t>
+  </si>
+  <si>
+    <t>Louisiana</t>
+  </si>
+  <si>
+    <t>Maine</t>
+  </si>
+  <si>
+    <t>Maryland</t>
+  </si>
+  <si>
+    <t>Massachusetts</t>
+  </si>
+  <si>
+    <t>Michigan</t>
+  </si>
+  <si>
+    <t>Minnesota</t>
+  </si>
+  <si>
+    <t>Mississippi</t>
+  </si>
+  <si>
+    <t>Missouri</t>
+  </si>
+  <si>
+    <t>Montana</t>
+  </si>
+  <si>
+    <t>Nebraska</t>
+  </si>
+  <si>
+    <t>Nevada</t>
+  </si>
+  <si>
+    <t>New Hampshire</t>
+  </si>
+  <si>
+    <t>New Jersey</t>
+  </si>
+  <si>
+    <t>New Mexico</t>
+  </si>
+  <si>
+    <t>New York</t>
+  </si>
+  <si>
+    <t>North Carolina</t>
+  </si>
+  <si>
+    <t>North Dakota</t>
+  </si>
+  <si>
+    <t>Ohio</t>
+  </si>
+  <si>
+    <t>Oklahoma</t>
+  </si>
+  <si>
+    <t>Oregon</t>
+  </si>
+  <si>
+    <t>Pennsylvania</t>
+  </si>
+  <si>
+    <t>Rhode Island</t>
+  </si>
+  <si>
+    <t>South Carolina</t>
+  </si>
+  <si>
+    <t>South Dakota</t>
+  </si>
+  <si>
+    <t>Tennessee</t>
+  </si>
+  <si>
+    <t>Texas</t>
+  </si>
+  <si>
+    <t>Utah</t>
+  </si>
+  <si>
+    <t>Vermont</t>
+  </si>
+  <si>
+    <t>Virginia</t>
+  </si>
+  <si>
+    <t>Washington</t>
+  </si>
+  <si>
+    <t>West Virginia</t>
+  </si>
+  <si>
+    <t>Wisconsin</t>
+  </si>
+  <si>
+    <t>Wyoming</t>
+  </si>
+  <si>
+    <t>New England</t>
+  </si>
+  <si>
+    <t>Mideast</t>
+  </si>
+  <si>
+    <t>Great Lakes</t>
+  </si>
+  <si>
+    <t>Plains</t>
+  </si>
+  <si>
+    <t>Southeast</t>
+  </si>
+  <si>
+    <t>Southwest</t>
+  </si>
+  <si>
+    <t>Rocky Mountain</t>
+  </si>
+  <si>
+    <t>Far West</t>
+  </si>
+  <si>
+    <t>Legend / Footnotes:</t>
+  </si>
+  <si>
+    <t>Real GDP is in millions of chained 2012 dollars. Calculations are performed on unrounded data. Chained (2012) dollar series are calculated as the product of the chain-type quantity index and the 2012 current-dollar value of the corresponding series, divided by 100. Because the formula for the chain-type quantity indexes uses weights of more than one period, the corresponding chained-dollar estimates are usually not additive. The difference between the United States and sum-of-states reflects federal military and civilian activity located overseas, as well as the differences in source data used to estimate GDP by industry and the expenditures measure of real GDP.</t>
+  </si>
+  <si>
+    <t>Last updated: October 2, 2020-- revised statistics for 1997-2019.</t>
+  </si>
+  <si>
+    <t>AL</t>
+  </si>
+  <si>
+    <t>AK</t>
+  </si>
+  <si>
+    <t>AZ</t>
+  </si>
+  <si>
+    <t>AR</t>
+  </si>
+  <si>
+    <t>CA</t>
+  </si>
+  <si>
+    <t>CO</t>
+  </si>
+  <si>
+    <t>CT</t>
+  </si>
+  <si>
+    <t>DE</t>
+  </si>
+  <si>
+    <t>FL</t>
+  </si>
+  <si>
+    <t>GA</t>
+  </si>
+  <si>
+    <t>HI</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>IL</t>
+  </si>
+  <si>
+    <t>IN</t>
+  </si>
+  <si>
+    <t>IA</t>
+  </si>
+  <si>
+    <t>KS</t>
+  </si>
+  <si>
+    <t>KY</t>
+  </si>
+  <si>
+    <t>LA</t>
+  </si>
+  <si>
+    <t>ME</t>
+  </si>
+  <si>
+    <t>MD</t>
+  </si>
+  <si>
+    <t>MA</t>
+  </si>
+  <si>
+    <t>MI</t>
+  </si>
+  <si>
+    <t>MN</t>
+  </si>
+  <si>
+    <t>MS</t>
+  </si>
+  <si>
+    <t>MO</t>
+  </si>
+  <si>
+    <t>MT</t>
+  </si>
+  <si>
+    <t>NE</t>
+  </si>
+  <si>
+    <t>NV</t>
+  </si>
+  <si>
+    <t>NH</t>
+  </si>
+  <si>
+    <t>NJ</t>
+  </si>
+  <si>
+    <t>NM</t>
+  </si>
+  <si>
+    <t>NY</t>
+  </si>
+  <si>
+    <t>NC</t>
+  </si>
+  <si>
+    <t>ND</t>
+  </si>
+  <si>
+    <t>OH</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>OR</t>
+  </si>
+  <si>
+    <t>PA</t>
+  </si>
+  <si>
+    <t>RI</t>
+  </si>
+  <si>
+    <t>SC</t>
+  </si>
+  <si>
+    <t>SD</t>
+  </si>
+  <si>
+    <t>TN</t>
+  </si>
+  <si>
+    <t>TX</t>
+  </si>
+  <si>
+    <t>UT</t>
+  </si>
+  <si>
+    <t>VT</t>
+  </si>
+  <si>
+    <t>VA</t>
+  </si>
+  <si>
+    <t>WA</t>
+  </si>
+  <si>
+    <t>WV</t>
+  </si>
+  <si>
+    <t>WI</t>
+  </si>
+  <si>
+    <t>WY</t>
+  </si>
+  <si>
+    <t>State GDP</t>
+  </si>
+  <si>
+    <t>Bureau of Economic Analysis</t>
+  </si>
+  <si>
+    <t>State GDP Annual Data</t>
+  </si>
+  <si>
+    <t>State specific downscaling factor</t>
+  </si>
+  <si>
+    <t>State downscaling</t>
+  </si>
+  <si>
+    <t>Downcale DACD-potential is approximated based on the state's fraction of national GDP in 2019</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -334,6 +726,13 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF403F41"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -379,7 +778,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -402,6 +801,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -432,13 +835,19 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>265044</xdr:colOff>
+      <xdr:colOff>44174</xdr:colOff>
       <xdr:row>47</xdr:row>
       <xdr:rowOff>143350</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -476,13 +885,19 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>74543</xdr:colOff>
+      <xdr:colOff>74544</xdr:colOff>
       <xdr:row>32</xdr:row>
       <xdr:rowOff>43244</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -776,186 +1191,570 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.140625" customWidth="1"/>
-    <col min="2" max="2" width="47.140625" customWidth="1"/>
+    <col min="1" max="1" width="11.1640625" customWidth="1"/>
+    <col min="2" max="2" width="47.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>101</v>
+      </c>
+      <c r="J1" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="K1" s="19" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B2" t="str">
+        <f>LOOKUP(B1,J1:K50,K1:K50)</f>
+        <v>CO</v>
+      </c>
+      <c r="J2" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="K2" s="19" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J3" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="K3" s="19" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J4" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="K4" s="19" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J5" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="K5" s="19" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J6" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="K6" s="19" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B7" s="7">
         <v>2019</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J7" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="K7" s="19" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J8" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="K8" s="19" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B9" s="6" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J9" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="K9" s="19" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J10" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="K10" s="19" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B11" s="6" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J11" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="K11" s="19" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="J12" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="K12" s="19" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J13" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="K13" s="19" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B14" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="J14" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="K14" s="19" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>209</v>
+      </c>
+      <c r="J15" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="K15" s="19" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>210</v>
+      </c>
+      <c r="J16" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="K16" s="19" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B17" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="J17" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="K17" s="19" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J18" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="K18" s="19" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J19" s="19" t="s">
+        <v>115</v>
+      </c>
+      <c r="K19" s="19" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="J20" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="K20" s="19" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="J21" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="K21" s="19" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="J22" s="19" t="s">
+        <v>118</v>
+      </c>
+      <c r="K22" s="19" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="J23" s="19" t="s">
+        <v>119</v>
+      </c>
+      <c r="K23" s="19" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="J24" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="K24" s="19" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J25" s="19" t="s">
+        <v>121</v>
+      </c>
+      <c r="K25" s="19" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="J26" s="19" t="s">
+        <v>122</v>
+      </c>
+      <c r="K26" s="19" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="J27" s="19" t="s">
+        <v>123</v>
+      </c>
+      <c r="K27" s="19" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="J28" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="K28" s="19" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
+      <c r="J29" s="19" t="s">
+        <v>125</v>
+      </c>
+      <c r="K29" s="19" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J30" s="19" t="s">
+        <v>126</v>
+      </c>
+      <c r="K30" s="19" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="J31" s="19" t="s">
+        <v>127</v>
+      </c>
+      <c r="K31" s="19" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="J32" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="K32" s="19" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
         <v>85</v>
+      </c>
+      <c r="J33" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="K33" s="19" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J34" s="19" t="s">
+        <v>130</v>
+      </c>
+      <c r="K34" s="19" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="J35" s="19" t="s">
+        <v>131</v>
+      </c>
+      <c r="K35" s="19" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>213</v>
+      </c>
+      <c r="J36" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="K36" s="19" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J37" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="K37" s="19" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J38" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="K38" s="19" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J39" s="19" t="s">
+        <v>135</v>
+      </c>
+      <c r="K39" s="19" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J40" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="K40" s="19" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J41" s="19" t="s">
+        <v>137</v>
+      </c>
+      <c r="K41" s="19" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J42" s="19" t="s">
+        <v>138</v>
+      </c>
+      <c r="K42" s="19" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J43" s="19" t="s">
+        <v>139</v>
+      </c>
+      <c r="K43" s="19" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J44" s="19" t="s">
+        <v>140</v>
+      </c>
+      <c r="K44" s="19" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J45" s="19" t="s">
+        <v>141</v>
+      </c>
+      <c r="K45" s="19" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J46" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="K46" s="19" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J47" s="19" t="s">
+        <v>143</v>
+      </c>
+      <c r="K47" s="19" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J48" s="19" t="s">
+        <v>144</v>
+      </c>
+      <c r="K48" s="19" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="49" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J49" s="19" t="s">
+        <v>145</v>
+      </c>
+      <c r="K49" s="19" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="50" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J50" s="19" t="s">
+        <v>146</v>
+      </c>
+      <c r="K50" s="19" t="s">
+        <v>207</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B9" r:id="rId1"/>
-    <hyperlink ref="B11" r:id="rId2"/>
+    <hyperlink ref="B9" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B11" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B17" r:id="rId3" location="reqid=70&amp;step=1&amp;isuri=1 " xr:uid="{A879BB86-0F2A-204A-90E5-4D2B3F051D0B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H94"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A103" sqref="A103"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="33.28515625" customWidth="1"/>
-    <col min="2" max="8" width="11.42578125" customWidth="1"/>
+    <col min="1" max="1" width="36.1640625" customWidth="1"/>
+    <col min="2" max="8" width="11.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="4"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="16" t="s">
         <v>82</v>
       </c>
@@ -966,7 +1765,7 @@
       <c r="F8" s="17"/>
       <c r="G8" s="17"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>6</v>
       </c>
@@ -977,7 +1776,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>1</v>
       </c>
@@ -988,7 +1787,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>2</v>
       </c>
@@ -999,7 +1798,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>3</v>
       </c>
@@ -1010,12 +1809,12 @@
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>9</v>
       </c>
@@ -1026,7 +1825,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>1</v>
       </c>
@@ -1037,7 +1836,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>2</v>
       </c>
@@ -1048,17 +1847,17 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>9</v>
       </c>
@@ -1069,7 +1868,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>1</v>
       </c>
@@ -1080,7 +1879,7 @@
         <v>7.2</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>2</v>
       </c>
@@ -1091,32 +1890,32 @@
         <v>4.4000000000000004</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" s="5" t="s">
         <v>44</v>
       </c>
@@ -1128,27 +1927,27 @@
       <c r="G51" s="11"/>
       <c r="H51" s="11"/>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B57">
         <v>2045</v>
       </c>
@@ -1171,7 +1970,7 @@
         <v>2100</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>30</v>
       </c>
@@ -1197,7 +1996,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>31</v>
       </c>
@@ -1223,7 +2022,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>32</v>
       </c>
@@ -1231,7 +2030,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B63">
         <v>2045</v>
       </c>
@@ -1254,7 +2053,7 @@
         <v>2100</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>33</v>
       </c>
@@ -1287,7 +2086,7 @@
         <v>27.071428571428573</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>34</v>
       </c>
@@ -1320,27 +2119,27 @@
         <v>2.8571428571428568</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>39</v>
       </c>
@@ -1354,7 +2153,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>40</v>
       </c>
@@ -1368,7 +2167,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>43</v>
       </c>
@@ -1377,7 +2176,7 @@
         <v>0.24237500000000001</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" s="5" t="s">
         <v>45</v>
       </c>
@@ -1389,7 +2188,7 @@
       <c r="G76" s="11"/>
       <c r="H76" s="11"/>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B77">
         <v>2045</v>
       </c>
@@ -1412,7 +2211,7 @@
         <v>2100</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>33</v>
       </c>
@@ -1445,7 +2244,7 @@
         <v>6.5614375000000003</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>34</v>
       </c>
@@ -1478,12 +2277,12 @@
         <v>0.69249999999999989</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B82">
         <v>2045</v>
       </c>
@@ -1506,7 +2305,7 @@
         <v>2100</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>47</v>
       </c>
@@ -1539,7 +2338,7 @@
         <v>6561437500</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>48</v>
       </c>
@@ -1572,32 +2371,32 @@
         <v>692499999.99999988</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A86" s="5" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>55</v>
       </c>
@@ -1605,7 +2404,7 @@
         <v>947086</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>81</v>
       </c>
@@ -1618,21 +2417,1011 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CD1809B-8847-2543-BDEB-6EA7C8698DA1}">
+  <dimension ref="A1:D77"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="20" t="str">
+        <f>About!B1</f>
+        <v>Colorado</v>
+      </c>
+      <c r="B2" s="21">
+        <f>SUMIFS(D16:D74,B16:B74,A2)</f>
+        <v>1.8661560214087176E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>93</v>
+      </c>
+      <c r="B14" t="s">
+        <v>94</v>
+      </c>
+      <c r="C14">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>0</v>
+      </c>
+      <c r="B15" t="s">
+        <v>95</v>
+      </c>
+      <c r="C15">
+        <v>19091662</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>1000</v>
+      </c>
+      <c r="B16" t="s">
+        <v>96</v>
+      </c>
+      <c r="C16">
+        <v>200829.4</v>
+      </c>
+      <c r="D16" s="18">
+        <f t="shared" ref="D16:D47" si="0">C16/$C$15</f>
+        <v>1.0519220380080057E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>2000</v>
+      </c>
+      <c r="B17" t="s">
+        <v>97</v>
+      </c>
+      <c r="C17">
+        <v>53255.199999999997</v>
+      </c>
+      <c r="D17" s="18">
+        <f t="shared" si="0"/>
+        <v>2.7894480847188681E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>4000</v>
+      </c>
+      <c r="B18" t="s">
+        <v>98</v>
+      </c>
+      <c r="C18">
+        <v>323597.59999999998</v>
+      </c>
+      <c r="D18" s="18">
+        <f t="shared" si="0"/>
+        <v>1.6949682013016991E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>5000</v>
+      </c>
+      <c r="B19" t="s">
+        <v>99</v>
+      </c>
+      <c r="C19">
+        <v>117447.1</v>
+      </c>
+      <c r="D19" s="18">
+        <f t="shared" si="0"/>
+        <v>6.1517483391440725E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>6000</v>
+      </c>
+      <c r="B20" t="s">
+        <v>100</v>
+      </c>
+      <c r="C20">
+        <v>2800505.4</v>
+      </c>
+      <c r="D20" s="18">
+        <f t="shared" si="0"/>
+        <v>0.14668735493012602</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>8000</v>
+      </c>
+      <c r="B21" t="s">
+        <v>101</v>
+      </c>
+      <c r="C21">
+        <v>356280.2</v>
+      </c>
+      <c r="D21" s="18">
+        <f t="shared" si="0"/>
+        <v>1.8661560214087176E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>9000</v>
+      </c>
+      <c r="B22" t="s">
+        <v>102</v>
+      </c>
+      <c r="C22">
+        <v>251329.8</v>
+      </c>
+      <c r="D22" s="18">
+        <f t="shared" si="0"/>
+        <v>1.3164375107835032E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>10000</v>
+      </c>
+      <c r="B23" t="s">
+        <v>103</v>
+      </c>
+      <c r="C23">
+        <v>64319.3</v>
+      </c>
+      <c r="D23" s="18">
+        <f t="shared" si="0"/>
+        <v>3.3689733245853611E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>11000</v>
+      </c>
+      <c r="B24" t="s">
+        <v>104</v>
+      </c>
+      <c r="C24">
+        <v>123929.3</v>
+      </c>
+      <c r="D24" s="18">
+        <f t="shared" si="0"/>
+        <v>6.4912787582348782E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>12000</v>
+      </c>
+      <c r="B25" t="s">
+        <v>105</v>
+      </c>
+      <c r="C25">
+        <v>963255.9</v>
+      </c>
+      <c r="D25" s="18">
+        <f t="shared" si="0"/>
+        <v>5.0454271608202574E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>13000</v>
+      </c>
+      <c r="B26" t="s">
+        <v>106</v>
+      </c>
+      <c r="C26">
+        <v>547422.69999999995</v>
+      </c>
+      <c r="D26" s="18">
+        <f t="shared" si="0"/>
+        <v>2.8673391557005354E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>15000</v>
+      </c>
+      <c r="B27" t="s">
+        <v>107</v>
+      </c>
+      <c r="C27">
+        <v>82471.399999999994</v>
+      </c>
+      <c r="D27" s="18">
+        <f t="shared" si="0"/>
+        <v>4.3197601130797302E-3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>16000</v>
+      </c>
+      <c r="B28" t="s">
+        <v>108</v>
+      </c>
+      <c r="C28">
+        <v>74937.100000000006</v>
+      </c>
+      <c r="D28" s="18">
+        <f t="shared" si="0"/>
+        <v>3.9251218673366419E-3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>17000</v>
+      </c>
+      <c r="B29" t="s">
+        <v>109</v>
+      </c>
+      <c r="C29">
+        <v>773135.5</v>
+      </c>
+      <c r="D29" s="18">
+        <f t="shared" si="0"/>
+        <v>4.0495976725336953E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>18000</v>
+      </c>
+      <c r="B30" t="s">
+        <v>110</v>
+      </c>
+      <c r="C30">
+        <v>337636.1</v>
+      </c>
+      <c r="D30" s="18">
+        <f t="shared" si="0"/>
+        <v>1.7685003013357348E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>19000</v>
+      </c>
+      <c r="B31" t="s">
+        <v>111</v>
+      </c>
+      <c r="C31">
+        <v>173515.4</v>
+      </c>
+      <c r="D31" s="18">
+        <f t="shared" si="0"/>
+        <v>9.0885434699189624E-3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>20000</v>
+      </c>
+      <c r="B32" t="s">
+        <v>112</v>
+      </c>
+      <c r="C32">
+        <v>160059.29999999999</v>
+      </c>
+      <c r="D32" s="18">
+        <f t="shared" si="0"/>
+        <v>8.3837279331678925E-3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>21000</v>
+      </c>
+      <c r="B33" t="s">
+        <v>113</v>
+      </c>
+      <c r="C33">
+        <v>190811.5</v>
+      </c>
+      <c r="D33" s="18">
+        <f t="shared" si="0"/>
+        <v>9.9944939314345702E-3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>22000</v>
+      </c>
+      <c r="B34" t="s">
+        <v>114</v>
+      </c>
+      <c r="C34">
+        <v>239967.2</v>
+      </c>
+      <c r="D34" s="18">
+        <f t="shared" si="0"/>
+        <v>1.2569214770301297E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>23000</v>
+      </c>
+      <c r="B35" t="s">
+        <v>115</v>
+      </c>
+      <c r="C35">
+        <v>58793.3</v>
+      </c>
+      <c r="D35" s="18">
+        <f t="shared" si="0"/>
+        <v>3.0795275969163921E-3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>24000</v>
+      </c>
+      <c r="B36" t="s">
+        <v>116</v>
+      </c>
+      <c r="C36">
+        <v>374039.3</v>
+      </c>
+      <c r="D36" s="18">
+        <f t="shared" si="0"/>
+        <v>1.9591762100125174E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>25000</v>
+      </c>
+      <c r="B37" t="s">
+        <v>117</v>
+      </c>
+      <c r="C37">
+        <v>519961.59999999998</v>
+      </c>
+      <c r="D37" s="18">
+        <f t="shared" si="0"/>
+        <v>2.7235009712616953E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>26000</v>
+      </c>
+      <c r="B38" t="s">
+        <v>118</v>
+      </c>
+      <c r="C38">
+        <v>471648.1</v>
+      </c>
+      <c r="D38" s="18">
+        <f t="shared" si="0"/>
+        <v>2.4704402372093114E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>27000</v>
+      </c>
+      <c r="B39" t="s">
+        <v>119</v>
+      </c>
+      <c r="C39">
+        <v>341041.4</v>
+      </c>
+      <c r="D39" s="18">
+        <f t="shared" si="0"/>
+        <v>1.7863368836091905E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>28000</v>
+      </c>
+      <c r="B40" t="s">
+        <v>120</v>
+      </c>
+      <c r="C40">
+        <v>102656.4</v>
+      </c>
+      <c r="D40" s="18">
+        <f t="shared" si="0"/>
+        <v>5.3770279402599935E-3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>29000</v>
+      </c>
+      <c r="B41" t="s">
+        <v>121</v>
+      </c>
+      <c r="C41">
+        <v>287659.3</v>
+      </c>
+      <c r="D41" s="18">
+        <f t="shared" si="0"/>
+        <v>1.5067273870656206E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>30000</v>
+      </c>
+      <c r="B42" t="s">
+        <v>122</v>
+      </c>
+      <c r="C42">
+        <v>47916.3</v>
+      </c>
+      <c r="D42" s="18">
+        <f t="shared" si="0"/>
+        <v>2.5098024467435052E-3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>31000</v>
+      </c>
+      <c r="B43" t="s">
+        <v>123</v>
+      </c>
+      <c r="C43">
+        <v>117395.2</v>
+      </c>
+      <c r="D43" s="18">
+        <f t="shared" si="0"/>
+        <v>6.1490298749265516E-3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>32000</v>
+      </c>
+      <c r="B44" t="s">
+        <v>124</v>
+      </c>
+      <c r="C44">
+        <v>153728.6</v>
+      </c>
+      <c r="D44" s="18">
+        <f t="shared" si="0"/>
+        <v>8.0521329154056888E-3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>33000</v>
+      </c>
+      <c r="B45" t="s">
+        <v>125</v>
+      </c>
+      <c r="C45">
+        <v>77240.3</v>
+      </c>
+      <c r="D45" s="18">
+        <f t="shared" si="0"/>
+        <v>4.0457609190860389E-3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>34000</v>
+      </c>
+      <c r="B46" t="s">
+        <v>126</v>
+      </c>
+      <c r="C46">
+        <v>556731</v>
+      </c>
+      <c r="D46" s="18">
+        <f t="shared" si="0"/>
+        <v>2.9160949947678729E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>35000</v>
+      </c>
+      <c r="B47" t="s">
+        <v>127</v>
+      </c>
+      <c r="C47">
+        <v>98765.7</v>
+      </c>
+      <c r="D47" s="18">
+        <f t="shared" si="0"/>
+        <v>5.173237405941924E-3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>36000</v>
+      </c>
+      <c r="B48" t="s">
+        <v>128</v>
+      </c>
+      <c r="C48">
+        <v>1490678.5</v>
+      </c>
+      <c r="D48" s="18">
+        <f t="shared" ref="D48:D74" si="1">C48/$C$15</f>
+        <v>7.8080080194170634E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>37000</v>
+      </c>
+      <c r="B49" t="s">
+        <v>129</v>
+      </c>
+      <c r="C49">
+        <v>511539.9</v>
+      </c>
+      <c r="D49" s="18">
+        <f t="shared" si="1"/>
+        <v>2.679389044285406E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>38000</v>
+      </c>
+      <c r="B50" t="s">
+        <v>130</v>
+      </c>
+      <c r="C50">
+        <v>53930.2</v>
+      </c>
+      <c r="D50" s="18">
+        <f t="shared" si="1"/>
+        <v>2.8248038332126346E-3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>39000</v>
+      </c>
+      <c r="B51" t="s">
+        <v>131</v>
+      </c>
+      <c r="C51">
+        <v>615474.4</v>
+      </c>
+      <c r="D51" s="18">
+        <f t="shared" si="1"/>
+        <v>3.2237863838150915E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>40000</v>
+      </c>
+      <c r="B52" t="s">
+        <v>132</v>
+      </c>
+      <c r="C52">
+        <v>197900.4</v>
+      </c>
+      <c r="D52" s="18">
+        <f t="shared" si="1"/>
+        <v>1.036580262106044E-2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>41000</v>
+      </c>
+      <c r="B53" t="s">
+        <v>133</v>
+      </c>
+      <c r="C53">
+        <v>225336.8</v>
+      </c>
+      <c r="D53" s="18">
+        <f t="shared" si="1"/>
+        <v>1.1802890706948404E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>42000</v>
+      </c>
+      <c r="B54" t="s">
+        <v>134</v>
+      </c>
+      <c r="C54">
+        <v>726165.9</v>
+      </c>
+      <c r="D54" s="18">
+        <f t="shared" si="1"/>
+        <v>3.8035761370592044E-2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>44000</v>
+      </c>
+      <c r="B55" t="s">
+        <v>135</v>
+      </c>
+      <c r="C55">
+        <v>53668</v>
+      </c>
+      <c r="D55" s="18">
+        <f t="shared" si="1"/>
+        <v>2.8110700891310564E-3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>45000</v>
+      </c>
+      <c r="B56" t="s">
+        <v>136</v>
+      </c>
+      <c r="C56">
+        <v>214933.7</v>
+      </c>
+      <c r="D56" s="18">
+        <f t="shared" si="1"/>
+        <v>1.1257987911162476E-2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>46000</v>
+      </c>
+      <c r="B57" t="s">
+        <v>137</v>
+      </c>
+      <c r="C57">
+        <v>47559.7</v>
+      </c>
+      <c r="D57" s="18">
+        <f t="shared" si="1"/>
+        <v>2.4911241357614645E-3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>47000</v>
+      </c>
+      <c r="B58" t="s">
+        <v>138</v>
+      </c>
+      <c r="C58">
+        <v>328406.3</v>
+      </c>
+      <c r="D58" s="18">
+        <f t="shared" si="1"/>
+        <v>1.7201556365286582E-2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>48000</v>
+      </c>
+      <c r="B59" t="s">
+        <v>139</v>
+      </c>
+      <c r="C59">
+        <v>1764357.2</v>
+      </c>
+      <c r="D59" s="18">
+        <f t="shared" si="1"/>
+        <v>9.2415065802023938E-2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>49000</v>
+      </c>
+      <c r="B60" t="s">
+        <v>140</v>
+      </c>
+      <c r="C60">
+        <v>168792.7</v>
+      </c>
+      <c r="D60" s="18">
+        <f t="shared" si="1"/>
+        <v>8.8411737019019089E-3</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>50000</v>
+      </c>
+      <c r="B61" t="s">
+        <v>141</v>
+      </c>
+      <c r="C61">
+        <v>29806.2</v>
+      </c>
+      <c r="D61" s="18">
+        <f t="shared" si="1"/>
+        <v>1.5612155714887473E-3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>51000</v>
+      </c>
+      <c r="B62" t="s">
+        <v>142</v>
+      </c>
+      <c r="C62">
+        <v>489168.4</v>
+      </c>
+      <c r="D62" s="18">
+        <f t="shared" si="1"/>
+        <v>2.5622096179997323E-2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>53000</v>
+      </c>
+      <c r="B63" t="s">
+        <v>143</v>
+      </c>
+      <c r="C63">
+        <v>548686.69999999995</v>
+      </c>
+      <c r="D63" s="18">
+        <f t="shared" si="1"/>
+        <v>2.8739598469740349E-2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <v>54000</v>
+      </c>
+      <c r="B64" t="s">
+        <v>144</v>
+      </c>
+      <c r="C64">
+        <v>72340.399999999994</v>
+      </c>
+      <c r="D64" s="18">
+        <f t="shared" si="1"/>
+        <v>3.7891096123532876E-3</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A65">
+        <v>55000</v>
+      </c>
+      <c r="B65" t="s">
+        <v>145</v>
+      </c>
+      <c r="C65">
+        <v>308044.7</v>
+      </c>
+      <c r="D65" s="18">
+        <f t="shared" si="1"/>
+        <v>1.613503842672262E-2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A66">
+        <v>56000</v>
+      </c>
+      <c r="B66" t="s">
+        <v>146</v>
+      </c>
+      <c r="C66">
+        <v>39214</v>
+      </c>
+      <c r="D66" s="18">
+        <f t="shared" si="1"/>
+        <v>2.0539856613845352E-3</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A67">
+        <v>91000</v>
+      </c>
+      <c r="B67" t="s">
+        <v>147</v>
+      </c>
+      <c r="C67">
+        <v>990777.5</v>
+      </c>
+      <c r="D67" s="18">
+        <f t="shared" si="1"/>
+        <v>5.1895822375233755E-2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A68">
+        <v>92000</v>
+      </c>
+      <c r="B68" t="s">
+        <v>148</v>
+      </c>
+      <c r="C68">
+        <v>3336480.6</v>
+      </c>
+      <c r="D68" s="18">
+        <f t="shared" si="1"/>
+        <v>0.17476113918212044</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A69">
+        <v>93000</v>
+      </c>
+      <c r="B69" t="s">
+        <v>149</v>
+      </c>
+      <c r="C69">
+        <v>2505871.7999999998</v>
+      </c>
+      <c r="D69" s="18">
+        <f t="shared" si="1"/>
+        <v>0.1312547749902549</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A70">
+        <v>94000</v>
+      </c>
+      <c r="B70" t="s">
+        <v>150</v>
+      </c>
+      <c r="C70">
+        <v>1181310.3999999999</v>
+      </c>
+      <c r="D70" s="18">
+        <f t="shared" si="1"/>
+        <v>6.187572354884556E-2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A71">
+        <v>95000</v>
+      </c>
+      <c r="B71" t="s">
+        <v>151</v>
+      </c>
+      <c r="C71">
+        <v>3981051.8</v>
+      </c>
+      <c r="D71" s="18">
+        <f t="shared" si="1"/>
+        <v>0.20852306100956533</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A72">
+        <v>96000</v>
+      </c>
+      <c r="B72" t="s">
+        <v>152</v>
+      </c>
+      <c r="C72">
+        <v>2386060.9</v>
+      </c>
+      <c r="D72" s="18">
+        <f t="shared" si="1"/>
+        <v>0.12497921343882999</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A73">
+        <v>97000</v>
+      </c>
+      <c r="B73" t="s">
+        <v>153</v>
+      </c>
+      <c r="C73">
+        <v>687941.6</v>
+      </c>
+      <c r="D73" s="18">
+        <f t="shared" si="1"/>
+        <v>3.6033615093332368E-2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A74">
+        <v>98000</v>
+      </c>
+      <c r="B74" t="s">
+        <v>154</v>
+      </c>
+      <c r="C74">
+        <v>3864650.3</v>
+      </c>
+      <c r="D74" s="18">
+        <f t="shared" si="1"/>
+        <v>0.20242608003431026</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>155</v>
+      </c>
+      <c r="D75" s="18"/>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>156</v>
+      </c>
+      <c r="D76" s="18"/>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>157</v>
+      </c>
+      <c r="D77" s="18"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A8" r:id="rId1" location="reqid=70&amp;step=1&amp;isuri=1 " xr:uid="{84AF32A5-78A2-BE4B-96E0-53671D9D23A5}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="8" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:AI2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AE7" sqref="AE7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="19.83203125" customWidth="1"/>
+    <col min="2" max="2" width="9.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>49</v>
       </c>
@@ -1739,7 +3528,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>78</v>
       </c>
@@ -1832,24 +3621,24 @@
         <v>0</v>
       </c>
       <c r="AE2">
-        <f>TREND(Data!$B$83:$C$83,Data!$B$82:$C$82,AE$1)</f>
-        <v>17312500</v>
+        <f>TREND(Data!$B$83:$C$83,Data!$B$82:$C$82,AE$1)*'State Downscale'!B2</f>
+        <v>323078.26120638422</v>
       </c>
       <c r="AF2">
-        <f>TREND(Data!$B$83:$C$83,Data!$B$82:$C$82,AF$1)</f>
-        <v>34625000</v>
+        <f>TREND(Data!$B$83:$C$83,Data!$B$82:$C$82,AF$1)*'State Downscale'!B2</f>
+        <v>646156.52241276845</v>
       </c>
       <c r="AG2">
-        <f>TREND(Data!$B$83:$C$83,Data!$B$82:$C$82,AG$1)</f>
-        <v>51937500</v>
+        <f>TREND(Data!$B$83:$C$83,Data!$B$82:$C$82,AG$1)*'State Downscale'!B2</f>
+        <v>969234.78361915273</v>
       </c>
       <c r="AH2">
-        <f>TREND(Data!$B$83:$C$83,Data!$B$82:$C$82,AH$1)</f>
-        <v>69250000</v>
+        <f>TREND(Data!$B$83:$C$83,Data!$B$82:$C$82,AH$1)*'State Downscale'!B2</f>
+        <v>1292313.0448255369</v>
       </c>
       <c r="AI2">
-        <f>TREND(Data!$B$83:$C$83,Data!$B$82:$C$82,AI$1)</f>
-        <v>86562500</v>
+        <f>TREND(Data!$B$83:$C$83,Data!$B$82:$C$82,AI$1)*'State Downscale'!B2</f>
+        <v>1615391.3060319212</v>
       </c>
     </row>
   </sheetData>
@@ -1857,8 +3646,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <tabColor theme="8" tint="-0.249977111117893"/>
   </sheetPr>
@@ -1866,13 +3655,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.7109375" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="24.6640625" customWidth="1"/>
+    <col min="2" max="2" width="9.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>56</v>
       </c>
@@ -1979,7 +3768,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A2" s="15" t="s">
         <v>68</v>
       </c>
@@ -2120,7 +3909,7 @@
         <v>1704754.8</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A3" s="15" t="s">
         <v>69</v>
       </c>
@@ -2260,7 +4049,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A4" s="15" t="s">
         <v>70</v>
       </c>
@@ -2401,7 +4190,7 @@
         <v>7671396.5999999996</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A5" s="15" t="s">
         <v>71</v>
       </c>
@@ -2541,7 +4330,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A6" s="15" t="s">
         <v>72</v>
       </c>
@@ -2681,7 +4470,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A7" s="15" t="s">
         <v>73</v>
       </c>
@@ -2821,7 +4610,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A8" s="15" t="s">
         <v>74</v>
       </c>
@@ -2961,7 +4750,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A9" s="15" t="s">
         <v>75</v>
       </c>
@@ -3101,7 +4890,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A10" s="15" t="s">
         <v>76</v>
       </c>
@@ -3241,7 +5030,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A11" s="15" t="s">
         <v>77</v>
       </c>
@@ -3386,22 +5175,24 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <tabColor theme="8" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:AI2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.7109375" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="24.6640625" customWidth="1"/>
+    <col min="2" max="2" width="9.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>57</v>
       </c>
@@ -3508,7 +5299,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>58</v>
       </c>

</xml_diff>